<commit_message>
What if analysis done
</commit_message>
<xml_diff>
--- a/BI/Pracs/What_if_analysis.xlsx
+++ b/BI/Pracs/What_if_analysis.xlsx
@@ -1,30 +1,49 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BSCIT\TY\6TH SEM\TYIT-6TH-SEM\BI\Pracs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{630A53C0-6175-4660-8D98-5744CB6D3494}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Scenario Summary" sheetId="4" r:id="rId1"/>
-    <sheet name="Scenario Summary 2" sheetId="5" r:id="rId2"/>
-    <sheet name="Scenario Summary 3" sheetId="6" r:id="rId3"/>
-    <sheet name="Case 1- Sales" sheetId="1" r:id="rId4"/>
-    <sheet name="Case 1 continuation" sheetId="2" r:id="rId5"/>
-    <sheet name="Case 2- Investment plan" sheetId="3" r:id="rId6"/>
+    <sheet name="Scenario Summary" sheetId="4" state="hidden" r:id="rId1"/>
+    <sheet name="Scenario Summary 2" sheetId="5" state="hidden" r:id="rId2"/>
+    <sheet name="Case 1- Sales" sheetId="1" r:id="rId3"/>
+    <sheet name="Case 1 continuation" sheetId="2" r:id="rId4"/>
+    <sheet name="Case 1 Summary" sheetId="6" r:id="rId5"/>
+    <sheet name="Scenario Summary 5" sheetId="8" state="hidden" r:id="rId6"/>
+    <sheet name="Case 2- Investment plan" sheetId="3" r:id="rId7"/>
+    <sheet name="Case 2 Summary" sheetId="7" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Lenovo</author>
   </authors>
   <commentList>
-    <comment ref="A10" authorId="0">
+    <comment ref="A10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
       <text>
         <r>
           <rPr>
@@ -54,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="72">
   <si>
     <t>Price</t>
   </si>
@@ -178,12 +197,6 @@
     <t>Total Investment</t>
   </si>
   <si>
-    <t>Total Quantity</t>
-  </si>
-  <si>
-    <t>Expected Returns</t>
-  </si>
-  <si>
     <t>No.Of Years</t>
   </si>
   <si>
@@ -200,16 +213,94 @@
   </si>
   <si>
     <t>Interest Rate</t>
+  </si>
+  <si>
+    <t>Maturity Amount</t>
+  </si>
+  <si>
+    <t>Interest Gained</t>
+  </si>
+  <si>
+    <t>TOTAL YEARS</t>
+  </si>
+  <si>
+    <t>PRINCIPAL AMOUNT INVESTED(ICICI BANK)</t>
+  </si>
+  <si>
+    <t>The data table gives the Maturity Amount when the Prinicpal Amount Invested vs Total Years the investment is made in ICICI Bank at a rate of interest of 15%</t>
+  </si>
+  <si>
+    <t>SCENARIO MANAGER</t>
+  </si>
+  <si>
+    <t>$B$33</t>
+  </si>
+  <si>
+    <t>$B$34</t>
+  </si>
+  <si>
+    <t>$B$35</t>
+  </si>
+  <si>
+    <t>$B$36</t>
+  </si>
+  <si>
+    <t>$D$33</t>
+  </si>
+  <si>
+    <t>$D$34</t>
+  </si>
+  <si>
+    <t>$D$35</t>
+  </si>
+  <si>
+    <t>$D$36</t>
+  </si>
+  <si>
+    <t>$F$33</t>
+  </si>
+  <si>
+    <t>$F$34</t>
+  </si>
+  <si>
+    <t>$F$35</t>
+  </si>
+  <si>
+    <t>$F$36</t>
+  </si>
+  <si>
+    <t>Scenario 1( P= 20,000, N=5)</t>
+  </si>
+  <si>
+    <t>Prinicpal amount invested is 20000 for 5 years with Simple interest</t>
+  </si>
+  <si>
+    <t>Scenario 2( P= 50,000, N=2)</t>
+  </si>
+  <si>
+    <t>Invest 50000 for 2 years with Simple Interest</t>
+  </si>
+  <si>
+    <t>Scenario 3( P= 60,000, N=3)</t>
+  </si>
+  <si>
+    <t>Invest 60000 for 3 years with Simple Interest</t>
+  </si>
+  <si>
+    <t>Scenario 4( P= 100,000, N=10)</t>
+  </si>
+  <si>
+    <t>Invest 1,00,000 for 10 years with Simple Interest</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="166" formatCode="&quot;₹&quot;\ #,##0.00"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -327,7 +418,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -343,12 +434,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -394,6 +479,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="18">
     <border>
@@ -621,14 +718,44 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -644,48 +771,17 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -696,25 +792,58 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="0" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -722,13 +851,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -766,7 +903,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -800,6 +937,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -834,9 +972,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1009,7 +1148,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -1019,222 +1158,221 @@
       <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="1"/>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="5.28515625" customWidth="1"/>
-    <col min="4" max="9" width="18.7109375" bestFit="1" customWidth="1" outlineLevel="1"/>
+    <col min="3" max="3" width="5.33203125" customWidth="1"/>
+    <col min="4" max="9" width="18.6640625" bestFit="1" customWidth="1" outlineLevel="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="15.75" thickBot="1"/>
-    <row r="2" spans="2:9" ht="15.75">
-      <c r="B2" s="20" t="s">
+    <row r="1" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B2" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-    </row>
-    <row r="3" spans="2:9" ht="15.75" collapsed="1">
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="26" t="s">
+      <c r="C2" s="7"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+    </row>
+    <row r="3" spans="2:9" ht="15.6" collapsed="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="26" t="s">
+      <c r="E3" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="26" t="s">
+      <c r="F3" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="26" t="s">
+      <c r="G3" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="26" t="s">
+      <c r="H3" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="26" t="s">
+      <c r="I3" s="13" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="2:9" ht="33.75" hidden="1" outlineLevel="1">
-      <c r="B4" s="22"/>
-      <c r="C4" s="22"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="28" t="s">
+    <row r="4" spans="2:9" ht="30.6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="E4" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="28" t="s">
+      <c r="F4" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="28" t="s">
+      <c r="G4" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="28" t="s">
+      <c r="H4" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="I4" s="28" t="s">
+      <c r="I4" s="15" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="2:9">
-      <c r="B5" s="23" t="s">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B5" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="23"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="21"/>
-    </row>
-    <row r="6" spans="2:9" outlineLevel="1">
-      <c r="B6" s="22"/>
-      <c r="C6" s="22" t="s">
+      <c r="C5" s="10"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+    </row>
+    <row r="6" spans="2:9" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="9"/>
+      <c r="C6" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="D6" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="27" t="s">
+      <c r="E6" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="27" t="s">
+      <c r="F6" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="G6" s="27" t="s">
+      <c r="G6" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="H6" s="27" t="s">
+      <c r="H6" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="I6" s="27" t="s">
+      <c r="I6" s="14" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="2:9" outlineLevel="1">
-      <c r="B7" s="22"/>
-      <c r="C7" s="22" t="s">
+    <row r="7" spans="2:9" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="9"/>
+      <c r="C7" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="17">
+      <c r="D7">
         <v>100</v>
       </c>
-      <c r="E7" s="27">
+      <c r="E7" s="14">
         <v>200</v>
       </c>
-      <c r="F7" s="27">
+      <c r="F7" s="14">
         <v>200</v>
       </c>
-      <c r="G7" s="27">
+      <c r="G7" s="14">
         <v>300</v>
       </c>
-      <c r="H7" s="27">
+      <c r="H7" s="14">
         <v>400</v>
       </c>
-      <c r="I7" s="27">
+      <c r="I7" s="14">
         <v>500</v>
       </c>
     </row>
-    <row r="8" spans="2:9" outlineLevel="1">
-      <c r="B8" s="22"/>
-      <c r="C8" s="22" t="s">
+    <row r="8" spans="2:9" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="9"/>
+      <c r="C8" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="17" t="s">
+      <c r="D8" t="s">
         <v>0</v>
       </c>
-      <c r="E8" s="27" t="s">
+      <c r="E8" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="F8" s="27" t="s">
+      <c r="F8" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="G8" s="27" t="s">
+      <c r="G8" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="H8" s="27" t="s">
+      <c r="H8" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="I8" s="27" t="s">
+      <c r="I8" s="14" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:9" outlineLevel="1">
-      <c r="B9" s="22"/>
-      <c r="C9" s="22" t="s">
+    <row r="9" spans="2:9" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="9"/>
+      <c r="C9" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="17">
+      <c r="D9">
         <v>505</v>
       </c>
-      <c r="E9" s="27">
+      <c r="E9" s="14">
         <v>50</v>
       </c>
-      <c r="F9" s="27">
+      <c r="F9" s="14">
         <v>100</v>
       </c>
-      <c r="G9" s="27">
+      <c r="G9" s="14">
         <v>250</v>
       </c>
-      <c r="H9" s="27">
+      <c r="H9" s="14">
         <v>50</v>
       </c>
-      <c r="I9" s="27">
+      <c r="I9" s="14">
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="2:9">
-      <c r="B10" s="23" t="s">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B10" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="23"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="21"/>
-      <c r="I10" s="21"/>
-    </row>
-    <row r="11" spans="2:9" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="B11" s="24"/>
-      <c r="C11" s="24" t="s">
+      <c r="C10" s="10"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+    </row>
+    <row r="11" spans="2:9" ht="15" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="11"/>
+      <c r="C11" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="18">
+      <c r="D11" s="5">
         <v>50500</v>
       </c>
-      <c r="E11" s="18">
+      <c r="E11" s="5">
         <v>10000</v>
       </c>
-      <c r="F11" s="18">
+      <c r="F11" s="5">
         <v>20000</v>
       </c>
-      <c r="G11" s="18">
+      <c r="G11" s="5">
         <v>75000</v>
       </c>
-      <c r="H11" s="18">
+      <c r="H11" s="5">
         <v>20000</v>
       </c>
-      <c r="I11" s="18">
+      <c r="I11" s="5">
         <v>20000</v>
       </c>
     </row>
-    <row r="12" spans="2:9">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="2:9">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="2:9">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>28</v>
       </c>
@@ -1245,7 +1383,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -1255,276 +1393,263 @@
       <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="1"/>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="5.28515625" customWidth="1"/>
-    <col min="4" max="10" width="18.7109375" bestFit="1" customWidth="1" outlineLevel="1"/>
+    <col min="3" max="3" width="5.33203125" customWidth="1"/>
+    <col min="4" max="10" width="18.6640625" bestFit="1" customWidth="1" outlineLevel="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="15.75" thickBot="1"/>
-    <row r="2" spans="2:10" ht="15.75">
-      <c r="B2" s="20" t="s">
+    <row r="1" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B2" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
-    </row>
-    <row r="3" spans="2:10" ht="15.75" collapsed="1">
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="26" t="s">
+      <c r="C2" s="7"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+    </row>
+    <row r="3" spans="2:10" ht="15.6" collapsed="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="26" t="s">
+      <c r="E3" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="26" t="s">
+      <c r="F3" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="26" t="s">
+      <c r="G3" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="26" t="s">
+      <c r="H3" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="26" t="s">
+      <c r="I3" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="J3" s="26" t="s">
+      <c r="J3" s="13" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="2:10" ht="56.25" hidden="1" outlineLevel="1">
-      <c r="B4" s="22"/>
-      <c r="C4" s="22"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="28" t="s">
+    <row r="4" spans="2:10" ht="51" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="E4" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="F4" s="28" t="s">
+      <c r="F4" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="28" t="s">
+      <c r="G4" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="28" t="s">
+      <c r="H4" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="I4" s="28" t="s">
+      <c r="I4" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="J4" s="28" t="s">
+      <c r="J4" s="15" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="2:10">
-      <c r="B5" s="23" t="s">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B5" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="23"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="21"/>
-      <c r="J5" s="21"/>
-    </row>
-    <row r="6" spans="2:10" outlineLevel="1">
-      <c r="B6" s="22"/>
-      <c r="C6" s="22" t="s">
+      <c r="C5" s="10"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+    </row>
+    <row r="6" spans="2:10" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="9"/>
+      <c r="C6" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="D6" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="27" t="s">
+      <c r="E6" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="27" t="s">
+      <c r="F6" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="G6" s="27" t="s">
+      <c r="G6" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="H6" s="27" t="s">
+      <c r="H6" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="I6" s="27" t="s">
+      <c r="I6" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="J6" s="17" t="s">
+      <c r="J6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="2:10" outlineLevel="1">
-      <c r="B7" s="22"/>
-      <c r="C7" s="22" t="s">
+    <row r="7" spans="2:10" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="9"/>
+      <c r="C7" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="17">
+      <c r="D7">
         <v>100</v>
       </c>
-      <c r="E7" s="27">
+      <c r="E7" s="14">
         <v>250</v>
       </c>
-      <c r="F7" s="27">
+      <c r="F7" s="14">
         <v>200</v>
       </c>
-      <c r="G7" s="27">
+      <c r="G7" s="14">
         <v>300</v>
       </c>
-      <c r="H7" s="27">
+      <c r="H7" s="14">
         <v>400</v>
       </c>
-      <c r="I7" s="27">
+      <c r="I7" s="14">
         <v>500</v>
       </c>
-      <c r="J7" s="27" t="s">
+      <c r="J7" s="14" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="2:10" outlineLevel="1">
-      <c r="B8" s="22"/>
-      <c r="C8" s="22" t="s">
+    <row r="8" spans="2:10" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="9"/>
+      <c r="C8" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="17" t="s">
+      <c r="D8" t="s">
         <v>0</v>
       </c>
-      <c r="E8" s="27" t="s">
+      <c r="E8" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="F8" s="27" t="s">
+      <c r="F8" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="G8" s="27" t="s">
+      <c r="G8" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="H8" s="27" t="s">
+      <c r="H8" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="I8" s="27" t="s">
+      <c r="I8" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="J8" s="17" t="s">
+      <c r="J8" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:10" outlineLevel="1">
-      <c r="B9" s="22"/>
-      <c r="C9" s="22" t="s">
+    <row r="9" spans="2:10" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="9"/>
+      <c r="C9" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="17">
+      <c r="D9">
         <v>505</v>
       </c>
-      <c r="E9" s="27">
+      <c r="E9" s="14">
         <v>50</v>
       </c>
-      <c r="F9" s="27">
+      <c r="F9" s="14">
         <v>100</v>
       </c>
-      <c r="G9" s="27">
+      <c r="G9" s="14">
         <v>250</v>
       </c>
-      <c r="H9" s="27">
+      <c r="H9" s="14">
         <v>50</v>
       </c>
-      <c r="I9" s="27">
+      <c r="I9" s="14">
         <v>40</v>
       </c>
-      <c r="J9" s="27" t="s">
+      <c r="J9" s="14" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:10" outlineLevel="1">
-      <c r="B10" s="22"/>
-      <c r="C10" s="22" t="s">
+    <row r="10" spans="2:10" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="9"/>
+      <c r="C10" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="27">
+      <c r="J10" s="14">
         <v>1000</v>
       </c>
     </row>
-    <row r="11" spans="2:10" outlineLevel="1">
-      <c r="B11" s="22"/>
-      <c r="C11" s="22" t="s">
+    <row r="11" spans="2:10" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="9"/>
+      <c r="C11" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="17"/>
-      <c r="J11" s="27">
+      <c r="J11" s="14">
         <v>235</v>
       </c>
     </row>
-    <row r="12" spans="2:10">
-      <c r="B12" s="23" t="s">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B12" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="23"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="21"/>
-      <c r="I12" s="21"/>
-      <c r="J12" s="21"/>
-    </row>
-    <row r="13" spans="2:10" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="B13" s="24"/>
-      <c r="C13" s="24" t="s">
+      <c r="C12" s="10"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+    </row>
+    <row r="13" spans="2:10" ht="15" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="11"/>
+      <c r="C13" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="18">
+      <c r="D13" s="5">
         <v>50500</v>
       </c>
-      <c r="E13" s="18">
+      <c r="E13" s="5">
         <v>12500</v>
       </c>
-      <c r="F13" s="18">
+      <c r="F13" s="5">
         <v>20000</v>
       </c>
-      <c r="G13" s="18">
+      <c r="G13" s="5">
         <v>75000</v>
       </c>
-      <c r="H13" s="18">
+      <c r="H13" s="5">
         <v>20000</v>
       </c>
-      <c r="I13" s="18">
+      <c r="I13" s="5">
         <v>20000</v>
       </c>
-      <c r="J13" s="18" t="e">
+      <c r="J13" s="5" t="e">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="14" spans="2:10">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="2:10">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="2:10">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>28</v>
       </c>
@@ -1535,288 +1660,28 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="B1:J14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="1"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="5.28515625" customWidth="1"/>
-    <col min="4" max="10" width="18.7109375" bestFit="1" customWidth="1" outlineLevel="1"/>
+    <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="64.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="15.75" thickBot="1"/>
-    <row r="2" spans="2:10" ht="15.75">
-      <c r="B2" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
-    </row>
-    <row r="3" spans="2:10" ht="15.75" collapsed="1">
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="26" t="s">
-        <v>24</v>
-      </c>
-      <c r="E3" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="J3" s="26" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="2:10" ht="56.25" hidden="1" outlineLevel="1">
-      <c r="B4" s="22"/>
-      <c r="C4" s="22"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="F4" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="H4" s="28" t="s">
-        <v>19</v>
-      </c>
-      <c r="I4" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="J4" s="28" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="2:10">
-      <c r="B5" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="23"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="21"/>
-      <c r="J5" s="21"/>
-    </row>
-    <row r="6" spans="2:10" outlineLevel="1">
-      <c r="B6" s="22"/>
-      <c r="C6" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="E6" s="27" t="s">
-        <v>2</v>
-      </c>
-      <c r="F6" s="27" t="s">
-        <v>2</v>
-      </c>
-      <c r="G6" s="27" t="s">
-        <v>2</v>
-      </c>
-      <c r="H6" s="27" t="s">
-        <v>2</v>
-      </c>
-      <c r="I6" s="27" t="s">
-        <v>2</v>
-      </c>
-      <c r="J6" s="27" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10" outlineLevel="1">
-      <c r="B7" s="22"/>
-      <c r="C7" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="17">
-        <v>100</v>
-      </c>
-      <c r="E7" s="27">
-        <v>250</v>
-      </c>
-      <c r="F7" s="27">
-        <v>200</v>
-      </c>
-      <c r="G7" s="27">
-        <v>300</v>
-      </c>
-      <c r="H7" s="27">
-        <v>400</v>
-      </c>
-      <c r="I7" s="27">
-        <v>500</v>
-      </c>
-      <c r="J7" s="27">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="8" spans="2:10" outlineLevel="1">
-      <c r="B8" s="22"/>
-      <c r="C8" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="E8" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="F8" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="G8" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="H8" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="I8" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="J8" s="27" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="2:10" outlineLevel="1">
-      <c r="B9" s="22"/>
-      <c r="C9" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="17">
-        <v>505</v>
-      </c>
-      <c r="E9" s="27">
-        <v>50</v>
-      </c>
-      <c r="F9" s="27">
-        <v>100</v>
-      </c>
-      <c r="G9" s="27">
-        <v>250</v>
-      </c>
-      <c r="H9" s="27">
-        <v>50</v>
-      </c>
-      <c r="I9" s="27">
-        <v>40</v>
-      </c>
-      <c r="J9" s="27">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="10" spans="2:10">
-      <c r="B10" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="23"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="21"/>
-      <c r="I10" s="21"/>
-      <c r="J10" s="21"/>
-    </row>
-    <row r="11" spans="2:10" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="B11" s="24"/>
-      <c r="C11" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="18">
-        <v>50500</v>
-      </c>
-      <c r="E11" s="18">
-        <v>12500</v>
-      </c>
-      <c r="F11" s="18">
-        <v>20000</v>
-      </c>
-      <c r="G11" s="18">
-        <v>75000</v>
-      </c>
-      <c r="H11" s="18">
-        <v>20000</v>
-      </c>
-      <c r="I11" s="18">
-        <v>20000</v>
-      </c>
-      <c r="J11" s="18">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="12" spans="2:10">
-      <c r="B12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="2:10">
-      <c r="B13" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="2:10">
-      <c r="B14" t="s">
-        <v>28</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L28"/>
-  <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="64.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" ht="15.75" thickBot="1"/>
-    <row r="2" spans="1:12" ht="28.5">
-      <c r="A2" s="10" t="s">
+    <row r="1" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:12" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-    </row>
-    <row r="3" spans="1:12">
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1825,7 +1690,7 @@
       </c>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -1834,7 +1699,7 @@
       </c>
       <c r="C4" s="2"/>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
@@ -1844,63 +1709,63 @@
       </c>
       <c r="C5" s="2"/>
     </row>
-    <row r="8" spans="1:12" ht="15.75" thickBot="1"/>
-    <row r="9" spans="1:12" ht="29.25" thickBot="1">
-      <c r="A9" s="7" t="s">
+    <row r="8" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="9" spans="1:12" ht="29.4" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A9" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="9"/>
-    </row>
-    <row r="10" spans="1:12">
-      <c r="A10" s="4">
+      <c r="B9" s="22"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="22"/>
+      <c r="J9" s="22"/>
+      <c r="K9" s="23"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
         <f>B5</f>
         <v>50500</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10" s="4">
         <v>100</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="4">
         <v>200</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="4">
         <v>300</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="4">
         <v>400</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="4">
         <v>500</v>
       </c>
-      <c r="G10" s="5">
+      <c r="G10" s="4">
         <v>600</v>
       </c>
-      <c r="H10" s="5">
+      <c r="H10" s="4">
         <v>700</v>
       </c>
-      <c r="I10" s="5">
+      <c r="I10" s="4">
         <v>800</v>
       </c>
-      <c r="J10" s="5">
+      <c r="J10" s="4">
         <v>900</v>
       </c>
-      <c r="K10" s="5">
+      <c r="K10" s="4">
         <v>1000</v>
       </c>
       <c r="L10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
-      <c r="A11" s="3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
         <v>50</v>
       </c>
       <c r="B11" s="2">
@@ -1935,8 +1800,8 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
-      <c r="A12" s="3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
         <v>60</v>
       </c>
       <c r="B12" s="2">
@@ -1970,8 +1835,8 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
-      <c r="A13" s="3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
         <v>70</v>
       </c>
       <c r="B13" s="2">
@@ -2005,8 +1870,8 @@
         <v>70000</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
-      <c r="A14" s="3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
         <v>80</v>
       </c>
       <c r="B14" s="2">
@@ -2040,8 +1905,8 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
-      <c r="A15" s="3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" s="2">
         <v>90</v>
       </c>
       <c r="B15" s="2">
@@ -2075,8 +1940,8 @@
         <v>90000</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
-      <c r="A16" s="3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
         <v>100</v>
       </c>
       <c r="B16" s="2">
@@ -2110,8 +1975,8 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
-      <c r="A17" s="3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" s="2">
         <v>110</v>
       </c>
       <c r="B17" s="2">
@@ -2145,8 +2010,8 @@
         <v>110000</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
-      <c r="A18" s="3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" s="2">
         <v>120</v>
       </c>
       <c r="B18" s="2">
@@ -2180,8 +2045,8 @@
         <v>120000</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
-      <c r="A19" s="3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" s="2">
         <v>130</v>
       </c>
       <c r="B19" s="2">
@@ -2215,8 +2080,8 @@
         <v>130000</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
-      <c r="A20" s="3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20" s="2">
         <v>140</v>
       </c>
       <c r="B20" s="2">
@@ -2250,8 +2115,8 @@
         <v>140000</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
-      <c r="A21" s="3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" s="2">
         <v>150</v>
       </c>
       <c r="B21" s="2">
@@ -2285,8 +2150,8 @@
         <v>150000</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
-      <c r="A22" s="3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22" s="2">
         <v>160</v>
       </c>
       <c r="B22" s="2">
@@ -2320,8 +2185,8 @@
         <v>160000</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
-      <c r="A23" s="3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23" s="2">
         <v>170</v>
       </c>
       <c r="B23" s="2">
@@ -2355,27 +2220,29 @@
         <v>170000</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="15.75" thickBot="1"/>
-    <row r="27" spans="1:11" ht="32.25" thickBot="1">
-      <c r="A27" s="14"/>
-      <c r="B27" s="15"/>
-      <c r="C27" s="15"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="16"/>
-    </row>
-    <row r="28" spans="1:11">
+    <row r="26" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="27" spans="1:11" ht="31.8" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="A27" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="B27" s="27"/>
+      <c r="C27" s="27"/>
+      <c r="D27" s="27"/>
+      <c r="E27" s="28"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>36</v>
       </c>
     </row>
   </sheetData>
   <scenarios current="4" sqref="B5">
-    <scenario name="Scenario 1( Dec'2023)" locked="1" count="4" user="Lenovo" comment="Dont select the output row of &quot;Total sale&quot; in goal seek table&#10;Modified by Lenovo on 1/13/2024">
+    <scenario name="Scenario 1( Dec'2023)" locked="1" count="4" user="Lenovo" comment="Dont select the output row of &quot;Total sale&quot; in goal seek table_x000a_Modified by Lenovo on 1/13/2024">
       <inputCells r="A3" val="No of items"/>
       <inputCells r="B3" val="250"/>
       <inputCells r="A4" val="Price"/>
@@ -2405,7 +2272,7 @@
       <inputCells r="A4" val="Price"/>
       <inputCells r="B4" val="40"/>
     </scenario>
-    <scenario name="Scenario 5(April'24)" locked="1" count="4" user="Lenovo" comment="April values&#10;Modified by Lenovo on 1/13/2024">
+    <scenario name="Scenario 5(April'24)" locked="1" count="4" user="Lenovo" comment="April values_x000a_Modified by Lenovo on 1/13/2024">
       <inputCells r="A3" val="No of items"/>
       <inputCells r="B3" val="200"/>
       <inputCells r="A4" val="Price"/>
@@ -2423,29 +2290,29 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" thickBot="1"/>
-    <row r="2" spans="1:3" ht="28.5">
-      <c r="A2" s="29" t="s">
+    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="31"/>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="B2" s="31"/>
+      <c r="C2" s="32"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -2454,7 +2321,7 @@
       </c>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -2463,7 +2330,7 @@
       </c>
       <c r="C4" s="2"/>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
@@ -2473,30 +2340,30 @@
       </c>
       <c r="C5" s="2"/>
     </row>
-    <row r="6" spans="1:3" ht="15.75" thickBot="1"/>
-    <row r="7" spans="1:3" ht="29.25" thickBot="1">
-      <c r="A7" s="32"/>
-      <c r="B7" s="32"/>
-      <c r="C7" s="32"/>
-    </row>
-    <row r="8" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A8" s="33"/>
-      <c r="B8" s="34"/>
-      <c r="C8" s="34"/>
-    </row>
-    <row r="9" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A9" s="33"/>
-      <c r="B9" s="34"/>
-      <c r="C9" s="34"/>
-    </row>
-    <row r="10" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A10" s="33"/>
-      <c r="B10" s="34"/>
-      <c r="C10" s="34"/>
+    <row r="6" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="7" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A7" s="29"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="29"/>
+    </row>
+    <row r="8" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="16"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+    </row>
+    <row r="9" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="16"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+    </row>
+    <row r="10" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="16"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
     </row>
   </sheetData>
   <scenarios current="0">
-    <scenario name="Scenario 5(April'24)" locked="1" count="4" user="Lenovo" comment="April values&#10;Modified by Lenovo on 1/13/2024">
+    <scenario name="Scenario 5(April'24)" locked="1" count="4" user="Lenovo" comment="April values_x000a_Modified by Lenovo on 1/13/2024">
       <inputCells r="A3" val="No of items"/>
       <inputCells r="B3" val="200"/>
       <inputCells r="A4" val="Price"/>
@@ -2511,180 +2378,1520 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="B1:J14"/>
+  <sheetViews>
+    <sheetView showGridLines="0" topLeftCell="G1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="5.33203125" customWidth="1"/>
+    <col min="4" max="10" width="18.6640625" bestFit="1" customWidth="1" outlineLevel="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B2" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+    </row>
+    <row r="3" spans="2:10" ht="15.6" collapsed="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" s="13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" ht="51" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="E4" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" s="15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B5" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="10"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+    </row>
+    <row r="6" spans="2:10" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="9"/>
+      <c r="C6" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="H6" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="I6" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="J6" s="14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="9"/>
+      <c r="C7" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7">
+        <v>100</v>
+      </c>
+      <c r="E7" s="14">
+        <v>250</v>
+      </c>
+      <c r="F7" s="14">
+        <v>200</v>
+      </c>
+      <c r="G7" s="14">
+        <v>300</v>
+      </c>
+      <c r="H7" s="14">
+        <v>400</v>
+      </c>
+      <c r="I7" s="14">
+        <v>500</v>
+      </c>
+      <c r="J7" s="14">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="9"/>
+      <c r="C8" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" t="s">
+        <v>0</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="G8" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="H8" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="I8" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="J8" s="14" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="9"/>
+      <c r="C9" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9">
+        <v>505</v>
+      </c>
+      <c r="E9" s="14">
+        <v>50</v>
+      </c>
+      <c r="F9" s="14">
+        <v>100</v>
+      </c>
+      <c r="G9" s="14">
+        <v>250</v>
+      </c>
+      <c r="H9" s="14">
+        <v>50</v>
+      </c>
+      <c r="I9" s="14">
+        <v>40</v>
+      </c>
+      <c r="J9" s="14">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B10" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="10"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+    </row>
+    <row r="11" spans="2:10" ht="15" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="11"/>
+      <c r="C11" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="5">
+        <v>50500</v>
+      </c>
+      <c r="E11" s="5">
+        <v>12500</v>
+      </c>
+      <c r="F11" s="5">
+        <v>20000</v>
+      </c>
+      <c r="G11" s="5">
+        <v>75000</v>
+      </c>
+      <c r="H11" s="5">
+        <v>20000</v>
+      </c>
+      <c r="I11" s="5">
+        <v>20000</v>
+      </c>
+      <c r="J11" s="5">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5B341A1-02C2-4644-AFC2-021192A45714}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="B1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:D14"/>
+    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="38.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="8" width="24.6640625" bestFit="1" customWidth="1" outlineLevel="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="39">
-      <c r="A1" s="35" t="s">
+    <row r="1" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B2" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+    </row>
+    <row r="3" spans="2:8" ht="15.6" collapsed="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" ht="20.399999999999999" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="53"/>
+      <c r="C4" s="53"/>
+      <c r="D4" s="49"/>
+      <c r="E4" s="56" t="s">
+        <v>65</v>
+      </c>
+      <c r="F4" s="56" t="s">
+        <v>67</v>
+      </c>
+      <c r="G4" s="56" t="s">
+        <v>69</v>
+      </c>
+      <c r="H4" s="56" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B5" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="10"/>
+      <c r="D5" s="52"/>
+      <c r="E5" s="52"/>
+      <c r="F5" s="52"/>
+      <c r="G5" s="52"/>
+      <c r="H5" s="52"/>
+    </row>
+    <row r="6" spans="2:8" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="53"/>
+      <c r="C6" s="53" t="s">
+        <v>52</v>
+      </c>
+      <c r="D6" s="50">
+        <v>100000</v>
+      </c>
+      <c r="E6" s="54">
+        <v>20000</v>
+      </c>
+      <c r="F6" s="54">
+        <v>50000</v>
+      </c>
+      <c r="G6" s="54">
+        <v>60000</v>
+      </c>
+      <c r="H6" s="54">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="53"/>
+      <c r="C7" s="53" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" s="50">
+        <v>100000</v>
+      </c>
+      <c r="E7" s="54">
+        <v>20000</v>
+      </c>
+      <c r="F7" s="54">
+        <v>50000</v>
+      </c>
+      <c r="G7" s="54">
+        <v>60000</v>
+      </c>
+      <c r="H7" s="54">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="53"/>
+      <c r="C8" s="53" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" s="50">
+        <v>100000</v>
+      </c>
+      <c r="E8" s="54">
+        <v>20000</v>
+      </c>
+      <c r="F8" s="54">
+        <v>50000</v>
+      </c>
+      <c r="G8" s="54">
+        <v>60000</v>
+      </c>
+      <c r="H8" s="54">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="53"/>
+      <c r="C9" s="53" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" s="50">
+        <v>100000</v>
+      </c>
+      <c r="E9" s="54">
+        <v>20000</v>
+      </c>
+      <c r="F9" s="54">
+        <v>50000</v>
+      </c>
+      <c r="G9" s="54">
+        <v>60000</v>
+      </c>
+      <c r="H9" s="54">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="53"/>
+      <c r="C10" s="53" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" s="49">
+        <v>10</v>
+      </c>
+      <c r="E10" s="55">
+        <v>5</v>
+      </c>
+      <c r="F10" s="55">
+        <v>2</v>
+      </c>
+      <c r="G10" s="55">
+        <v>4</v>
+      </c>
+      <c r="H10" s="55">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="53"/>
+      <c r="C11" s="53" t="s">
+        <v>57</v>
+      </c>
+      <c r="D11" s="49">
+        <v>10</v>
+      </c>
+      <c r="E11" s="55">
+        <v>5</v>
+      </c>
+      <c r="F11" s="55">
+        <v>2</v>
+      </c>
+      <c r="G11" s="55">
+        <v>4</v>
+      </c>
+      <c r="H11" s="55">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="53"/>
+      <c r="C12" s="53" t="s">
+        <v>58</v>
+      </c>
+      <c r="D12" s="49">
+        <v>10</v>
+      </c>
+      <c r="E12" s="55">
+        <v>5</v>
+      </c>
+      <c r="F12" s="55">
+        <v>2</v>
+      </c>
+      <c r="G12" s="55">
+        <v>4</v>
+      </c>
+      <c r="H12" s="55">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="53"/>
+      <c r="C13" s="53" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" s="49">
+        <v>10</v>
+      </c>
+      <c r="E13" s="55">
+        <v>5</v>
+      </c>
+      <c r="F13" s="55">
+        <v>2</v>
+      </c>
+      <c r="G13" s="55">
+        <v>4</v>
+      </c>
+      <c r="H13" s="55">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B14" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="10"/>
+      <c r="D14" s="52"/>
+      <c r="E14" s="52"/>
+      <c r="F14" s="52"/>
+      <c r="G14" s="52"/>
+      <c r="H14" s="52"/>
+    </row>
+    <row r="15" spans="2:8" ht="15" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="11"/>
+      <c r="C15" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="D15" s="51">
+        <v>250000</v>
+      </c>
+      <c r="E15" s="51">
+        <v>35000</v>
+      </c>
+      <c r="F15" s="51">
+        <v>65000</v>
+      </c>
+      <c r="G15" s="51">
+        <v>96000</v>
+      </c>
+      <c r="H15" s="51">
+        <v>250000</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:K36"/>
+  <sheetViews>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="38.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="15.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="38.4" x14ac:dyDescent="0.7">
+      <c r="A1" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="35"/>
-    </row>
-    <row r="5" spans="1:11" ht="28.5">
-      <c r="A5" s="36" t="s">
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="F3" s="18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="35">
+        <v>20000</v>
+      </c>
+      <c r="C4" s="20">
+        <v>0.15</v>
+      </c>
+      <c r="D4" s="19">
+        <v>2</v>
+      </c>
+      <c r="E4" s="35">
+        <f>C4*B4*D4</f>
+        <v>6000</v>
+      </c>
+      <c r="F4" s="35">
+        <f>B4+E4</f>
+        <v>26000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="35">
+        <v>6000</v>
+      </c>
+      <c r="C5" s="20">
+        <v>0.05</v>
+      </c>
+      <c r="D5" s="19">
+        <v>3</v>
+      </c>
+      <c r="E5" s="35">
+        <f t="shared" ref="E5:E7" si="0">C5*B5*D5</f>
+        <v>900</v>
+      </c>
+      <c r="F5" s="35">
+        <f t="shared" ref="F5:F7" si="1">B5+E5</f>
+        <v>6900</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="35">
+        <v>80000</v>
+      </c>
+      <c r="C6" s="20">
+        <v>0.2</v>
+      </c>
+      <c r="D6" s="19">
+        <v>5</v>
+      </c>
+      <c r="E6" s="35">
+        <f t="shared" si="0"/>
+        <v>80000</v>
+      </c>
+      <c r="F6" s="35">
+        <f t="shared" si="1"/>
+        <v>160000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="35">
+        <v>100000</v>
+      </c>
+      <c r="C7" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="D7" s="19">
+        <v>10</v>
+      </c>
+      <c r="E7" s="35">
+        <f t="shared" si="0"/>
+        <v>500000</v>
+      </c>
+      <c r="F7" s="35">
+        <f t="shared" si="1"/>
+        <v>600000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="9" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A9" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="36"/>
-      <c r="C5" s="36"/>
-      <c r="D5" s="36"/>
-      <c r="E5" s="36"/>
-    </row>
-    <row r="6" spans="1:11">
-      <c r="A6" s="37" t="s">
+      <c r="B9" s="37"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="38"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="B6" s="37" t="s">
+      <c r="B10" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="37" t="s">
+      <c r="C10" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="D6" s="37" t="s">
+      <c r="F10" s="18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="E6" s="37" t="s">
+      <c r="B11" s="35">
+        <v>30769.23076923077</v>
+      </c>
+      <c r="C11" s="20">
+        <v>0.15</v>
+      </c>
+      <c r="D11" s="19">
+        <v>2</v>
+      </c>
+      <c r="E11" s="35">
+        <f>C11*B11*D11</f>
+        <v>9230.7692307692305</v>
+      </c>
+      <c r="F11" s="35">
+        <f>B11+E11</f>
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" s="19" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="7" spans="1:11">
-      <c r="A7" s="38" t="s">
+      <c r="B12" s="35">
+        <v>47619.047619047618</v>
+      </c>
+      <c r="C12" s="20">
+        <v>0.05</v>
+      </c>
+      <c r="D12" s="19">
+        <v>3</v>
+      </c>
+      <c r="E12" s="35">
+        <f t="shared" ref="E12:E14" si="2">C12*B12*D12</f>
+        <v>7142.8571428571431</v>
+      </c>
+      <c r="F12" s="35">
+        <f t="shared" ref="F12:F14" si="3">B12+E12</f>
+        <v>54761.904761904763</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="B7" s="39">
+      <c r="B13" s="35">
+        <v>166666.66666666666</v>
+      </c>
+      <c r="C13" s="20">
+        <v>0.2</v>
+      </c>
+      <c r="D13" s="19">
+        <v>5</v>
+      </c>
+      <c r="E13" s="35">
+        <f t="shared" si="2"/>
+        <v>166666.66666666669</v>
+      </c>
+      <c r="F13" s="35">
+        <f t="shared" si="3"/>
+        <v>333333.33333333337</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" s="35">
+        <v>833333.33333333349</v>
+      </c>
+      <c r="C14" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="D14" s="19">
+        <v>10</v>
+      </c>
+      <c r="E14" s="35">
+        <f t="shared" si="2"/>
+        <v>4166666.6666666674</v>
+      </c>
+      <c r="F14" s="35">
+        <f t="shared" si="3"/>
+        <v>5000000.0000000009</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B15" s="34"/>
+      <c r="C15" s="34"/>
+      <c r="D15" s="34"/>
+    </row>
+    <row r="16" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="39"/>
+    </row>
+    <row r="17" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="41"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="41"/>
+      <c r="F17" s="42"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="43"/>
+      <c r="B18" s="44"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="39"/>
+      <c r="B19" s="45" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" s="45"/>
+      <c r="D19" s="45"/>
+      <c r="E19" s="45"/>
+      <c r="F19" s="45"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="46" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" s="48">
+        <f>F11</f>
+        <v>40000</v>
+      </c>
+      <c r="C20" s="48">
+        <v>10000</v>
+      </c>
+      <c r="D20" s="48">
+        <v>15000</v>
+      </c>
+      <c r="E20" s="48">
         <v>20000</v>
       </c>
-      <c r="C7" s="40">
+      <c r="F20" s="48">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="46"/>
+      <c r="B21" s="47">
+        <v>5</v>
+      </c>
+      <c r="C21" s="44">
+        <f t="dataTable" ref="C21:F26" dt2D="1" dtr="1" r1="B11" r2="D11"/>
+        <v>17500</v>
+      </c>
+      <c r="D21" s="44">
+        <v>26250</v>
+      </c>
+      <c r="E21" s="44">
+        <v>35000</v>
+      </c>
+      <c r="F21" s="44">
+        <v>52500</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="46"/>
+      <c r="B22" s="47">
+        <v>10</v>
+      </c>
+      <c r="C22" s="44">
+        <v>25000</v>
+      </c>
+      <c r="D22" s="44">
+        <v>37500</v>
+      </c>
+      <c r="E22" s="44">
+        <v>50000</v>
+      </c>
+      <c r="F22" s="44">
+        <v>75000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="46"/>
+      <c r="B23" s="47">
+        <v>15</v>
+      </c>
+      <c r="C23" s="44">
+        <v>32500</v>
+      </c>
+      <c r="D23" s="44">
+        <v>48750</v>
+      </c>
+      <c r="E23" s="44">
+        <v>65000</v>
+      </c>
+      <c r="F23" s="44">
+        <v>97500</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="46"/>
+      <c r="B24" s="47">
+        <v>20</v>
+      </c>
+      <c r="C24" s="44">
+        <v>40000</v>
+      </c>
+      <c r="D24" s="44">
+        <v>60000</v>
+      </c>
+      <c r="E24" s="44">
+        <v>80000</v>
+      </c>
+      <c r="F24" s="44">
+        <v>120000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="46"/>
+      <c r="B25" s="47">
+        <v>25</v>
+      </c>
+      <c r="C25" s="44">
+        <v>47500</v>
+      </c>
+      <c r="D25" s="44">
+        <v>71250</v>
+      </c>
+      <c r="E25" s="44">
+        <v>95000</v>
+      </c>
+      <c r="F25" s="44">
+        <v>142500</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="46"/>
+      <c r="B26" s="47">
+        <v>30</v>
+      </c>
+      <c r="C26" s="44">
+        <v>55000</v>
+      </c>
+      <c r="D26" s="44">
+        <v>82500</v>
+      </c>
+      <c r="E26" s="44">
+        <v>110000</v>
+      </c>
+      <c r="F26" s="44">
+        <v>165000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" s="34" t="s">
+        <v>50</v>
+      </c>
+      <c r="B28" s="34"/>
+      <c r="C28" s="34"/>
+      <c r="D28" s="34"/>
+      <c r="E28" s="34"/>
+      <c r="F28" s="34"/>
+    </row>
+    <row r="30" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="31" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A31" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="B31" s="37"/>
+      <c r="C31" s="37"/>
+      <c r="D31" s="37"/>
+      <c r="E31" s="37"/>
+      <c r="F31" s="38"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B32" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C32" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="D32" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="E32" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="F32" s="18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="B33" s="35">
+        <v>100000</v>
+      </c>
+      <c r="C33" s="20">
         <v>0.15</v>
       </c>
-      <c r="D7" s="39">
-        <f>C7*B7</f>
-        <v>3000</v>
-      </c>
-      <c r="E7" s="42">
+      <c r="D33" s="19">
+        <v>10</v>
+      </c>
+      <c r="E33" s="35">
+        <f>C33*B33*D33</f>
+        <v>150000</v>
+      </c>
+      <c r="F33" s="35">
+        <f>B33+E33</f>
+        <v>250000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="B34" s="35">
+        <v>100000</v>
+      </c>
+      <c r="C34" s="20">
+        <v>0.05</v>
+      </c>
+      <c r="D34" s="19">
+        <v>10</v>
+      </c>
+      <c r="E34" s="35">
+        <f t="shared" ref="E34:E36" si="4">C34*B34*D34</f>
+        <v>50000</v>
+      </c>
+      <c r="F34" s="35">
+        <f t="shared" ref="F34:F36" si="5">B34+E34</f>
+        <v>150000</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B35" s="35">
+        <v>100000</v>
+      </c>
+      <c r="C35" s="20">
+        <v>0.2</v>
+      </c>
+      <c r="D35" s="19">
+        <v>10</v>
+      </c>
+      <c r="E35" s="35">
+        <f t="shared" si="4"/>
+        <v>200000</v>
+      </c>
+      <c r="F35" s="35">
+        <f t="shared" si="5"/>
+        <v>300000</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="B36" s="35">
+        <v>100000</v>
+      </c>
+      <c r="C36" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="D36" s="19">
+        <v>10</v>
+      </c>
+      <c r="E36" s="35">
+        <f t="shared" si="4"/>
+        <v>500000</v>
+      </c>
+      <c r="F36" s="35">
+        <f t="shared" si="5"/>
+        <v>600000</v>
+      </c>
+    </row>
+  </sheetData>
+  <scenarios current="3" show="3" sqref="F33">
+    <scenario name="Scenario 1( P= 20,000, N=5)" locked="1" count="8" user="Aaditya Pal" comment="Prinicpal amount invested is 20000 for 5 years with Simple interest">
+      <inputCells r="B33" val="20000" numFmtId="166"/>
+      <inputCells r="B34" val="20000" numFmtId="166"/>
+      <inputCells r="B35" val="20000" numFmtId="166"/>
+      <inputCells r="B36" val="20000" numFmtId="166"/>
+      <inputCells r="D33" val="5"/>
+      <inputCells r="D34" val="5"/>
+      <inputCells r="D35" val="5"/>
+      <inputCells r="D36" val="5"/>
+    </scenario>
+    <scenario name="Scenario 2( P= 50,000, N=2)" locked="1" count="8" user="Aaditya Pal" comment="Invest 50000 for 2 years with Simple Interest">
+      <inputCells r="B33" val="50000" numFmtId="166"/>
+      <inputCells r="B34" val="50000" numFmtId="166"/>
+      <inputCells r="B35" val="50000" numFmtId="166"/>
+      <inputCells r="B36" val="50000" numFmtId="166"/>
+      <inputCells r="D33" val="2"/>
+      <inputCells r="D34" val="2"/>
+      <inputCells r="D35" val="2"/>
+      <inputCells r="D36" val="2"/>
+    </scenario>
+    <scenario name="Scenario 3( P= 60,000, N=3)" locked="1" count="8" user="Aaditya Pal" comment="Invest 60000 for 3 years with Simple Interest">
+      <inputCells r="B33" val="60000" numFmtId="166"/>
+      <inputCells r="B34" val="60000" numFmtId="166"/>
+      <inputCells r="B35" val="60000" numFmtId="166"/>
+      <inputCells r="B36" val="60000" numFmtId="166"/>
+      <inputCells r="D33" val="4"/>
+      <inputCells r="D34" val="4"/>
+      <inputCells r="D35" val="4"/>
+      <inputCells r="D36" val="4"/>
+    </scenario>
+    <scenario name="Scenario 4( P= 100,000, N=10)" locked="1" count="8" user="Aaditya Pal" comment="Invest 1,00,000 for 10 years with Simple Interest">
+      <inputCells r="B33" val="100000" numFmtId="166"/>
+      <inputCells r="B34" val="100000" numFmtId="166"/>
+      <inputCells r="B35" val="100000" numFmtId="166"/>
+      <inputCells r="B36" val="100000" numFmtId="166"/>
+      <inputCells r="D33" val="10"/>
+      <inputCells r="D34" val="10"/>
+      <inputCells r="D35" val="10"/>
+      <inputCells r="D36" val="10"/>
+    </scenario>
+  </scenarios>
+  <mergeCells count="8">
+    <mergeCell ref="A28:F28"/>
+    <mergeCell ref="A31:F31"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="A9:F9"/>
+    <mergeCell ref="A17:F17"/>
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="A20:A26"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{538A9CBF-08C1-40B4-A1E5-2F69D7660F51}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="B1:H21"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="6.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="8" width="24.6640625" customWidth="1" outlineLevel="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B2" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+    </row>
+    <row r="3" spans="2:8" ht="15.6" collapsed="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" ht="20.399999999999999" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="53"/>
+      <c r="C4" s="53"/>
+      <c r="D4" s="49"/>
+      <c r="E4" s="56" t="s">
+        <v>65</v>
+      </c>
+      <c r="F4" s="56" t="s">
+        <v>67</v>
+      </c>
+      <c r="G4" s="56" t="s">
+        <v>69</v>
+      </c>
+      <c r="H4" s="56" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B5" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="10"/>
+      <c r="D5" s="52"/>
+      <c r="E5" s="52"/>
+      <c r="F5" s="52"/>
+      <c r="G5" s="52"/>
+      <c r="H5" s="52"/>
+    </row>
+    <row r="6" spans="2:8" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="53"/>
+      <c r="C6" s="53" t="s">
+        <v>52</v>
+      </c>
+      <c r="D6" s="50">
+        <v>100000</v>
+      </c>
+      <c r="E6" s="54">
+        <v>20000</v>
+      </c>
+      <c r="F6" s="54">
+        <v>50000</v>
+      </c>
+      <c r="G6" s="54">
+        <v>60000</v>
+      </c>
+      <c r="H6" s="54">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="53"/>
+      <c r="C7" s="53" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" s="50">
+        <v>100000</v>
+      </c>
+      <c r="E7" s="54">
+        <v>20000</v>
+      </c>
+      <c r="F7" s="54">
+        <v>50000</v>
+      </c>
+      <c r="G7" s="54">
+        <v>60000</v>
+      </c>
+      <c r="H7" s="54">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="53"/>
+      <c r="C8" s="53" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" s="50">
+        <v>100000</v>
+      </c>
+      <c r="E8" s="54">
+        <v>20000</v>
+      </c>
+      <c r="F8" s="54">
+        <v>50000</v>
+      </c>
+      <c r="G8" s="54">
+        <v>60000</v>
+      </c>
+      <c r="H8" s="54">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="53"/>
+      <c r="C9" s="53" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" s="50">
+        <v>100000</v>
+      </c>
+      <c r="E9" s="54">
+        <v>20000</v>
+      </c>
+      <c r="F9" s="54">
+        <v>50000</v>
+      </c>
+      <c r="G9" s="54">
+        <v>60000</v>
+      </c>
+      <c r="H9" s="54">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="53"/>
+      <c r="C10" s="53" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" s="49">
+        <v>10</v>
+      </c>
+      <c r="E10" s="55">
+        <v>5</v>
+      </c>
+      <c r="F10" s="55">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:11">
-      <c r="A8" s="38" t="s">
-        <v>44</v>
-      </c>
-      <c r="B8" s="39">
-        <v>20000</v>
-      </c>
-      <c r="C8" s="40">
-        <v>0.05</v>
-      </c>
-      <c r="D8" s="39">
-        <f t="shared" ref="D8:D10" si="0">C8*B8</f>
-        <v>1000</v>
-      </c>
-      <c r="E8" s="42">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
-      <c r="A9" s="38" t="s">
-        <v>45</v>
-      </c>
-      <c r="B9" s="39">
-        <v>20000</v>
-      </c>
-      <c r="C9" s="40">
-        <v>0.2</v>
-      </c>
-      <c r="D9" s="39">
-        <f t="shared" si="0"/>
-        <v>4000</v>
-      </c>
-      <c r="E9" s="42">
+      <c r="G10" s="55">
+        <v>4</v>
+      </c>
+      <c r="H10" s="55">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="53"/>
+      <c r="C11" s="53" t="s">
+        <v>57</v>
+      </c>
+      <c r="D11" s="49">
+        <v>10</v>
+      </c>
+      <c r="E11" s="55">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:11">
-      <c r="A10" s="38" t="s">
-        <v>46</v>
-      </c>
-      <c r="B10" s="39">
-        <v>20000</v>
-      </c>
-      <c r="C10" s="40">
-        <v>0.5</v>
-      </c>
-      <c r="D10" s="39">
-        <f t="shared" si="0"/>
-        <v>10000</v>
-      </c>
-      <c r="E10" s="42">
+      <c r="F11" s="55">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" ht="28.5">
-      <c r="A14" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="B14" s="13"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-    </row>
-    <row r="15" spans="1:11">
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-    </row>
-    <row r="16" spans="1:11">
-      <c r="A16" s="41" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" s="41"/>
-    </row>
-    <row r="18" spans="1:1">
-      <c r="A18" s="41"/>
-    </row>
-    <row r="19" spans="1:1">
-      <c r="A19" s="41"/>
-    </row>
-    <row r="20" spans="1:1">
-      <c r="A20" s="41"/>
-    </row>
-    <row r="21" spans="1:1">
-      <c r="A21" s="41"/>
-    </row>
-    <row r="22" spans="1:1">
-      <c r="A22" s="41"/>
+      <c r="G11" s="55">
+        <v>4</v>
+      </c>
+      <c r="H11" s="55">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="53"/>
+      <c r="C12" s="53" t="s">
+        <v>58</v>
+      </c>
+      <c r="D12" s="49">
+        <v>10</v>
+      </c>
+      <c r="E12" s="55">
+        <v>5</v>
+      </c>
+      <c r="F12" s="55">
+        <v>2</v>
+      </c>
+      <c r="G12" s="55">
+        <v>4</v>
+      </c>
+      <c r="H12" s="55">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="53"/>
+      <c r="C13" s="53" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" s="49">
+        <v>10</v>
+      </c>
+      <c r="E13" s="55">
+        <v>5</v>
+      </c>
+      <c r="F13" s="55">
+        <v>2</v>
+      </c>
+      <c r="G13" s="55">
+        <v>4</v>
+      </c>
+      <c r="H13" s="55">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B14" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="10"/>
+      <c r="D14" s="52"/>
+      <c r="E14" s="52"/>
+      <c r="F14" s="52"/>
+      <c r="G14" s="52"/>
+      <c r="H14" s="52"/>
+    </row>
+    <row r="15" spans="2:8" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="53"/>
+      <c r="C15" s="53" t="s">
+        <v>60</v>
+      </c>
+      <c r="D15" s="50">
+        <v>250000</v>
+      </c>
+      <c r="E15" s="50">
+        <v>35000</v>
+      </c>
+      <c r="F15" s="50">
+        <v>65000</v>
+      </c>
+      <c r="G15" s="50">
+        <v>96000</v>
+      </c>
+      <c r="H15" s="50">
+        <v>250000</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="53"/>
+      <c r="C16" s="53" t="s">
+        <v>61</v>
+      </c>
+      <c r="D16" s="50">
+        <v>150000</v>
+      </c>
+      <c r="E16" s="50">
+        <v>25000</v>
+      </c>
+      <c r="F16" s="50">
+        <v>55000</v>
+      </c>
+      <c r="G16" s="50">
+        <v>72000</v>
+      </c>
+      <c r="H16" s="50">
+        <v>150000</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="53"/>
+      <c r="C17" s="53" t="s">
+        <v>62</v>
+      </c>
+      <c r="D17" s="50">
+        <v>300000</v>
+      </c>
+      <c r="E17" s="50">
+        <v>40000</v>
+      </c>
+      <c r="F17" s="50">
+        <v>70000</v>
+      </c>
+      <c r="G17" s="50">
+        <v>108000</v>
+      </c>
+      <c r="H17" s="50">
+        <v>300000</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" ht="15" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="11"/>
+      <c r="C18" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="D18" s="51">
+        <v>600000</v>
+      </c>
+      <c r="E18" s="51">
+        <v>70000</v>
+      </c>
+      <c r="F18" s="51">
+        <v>100000</v>
+      </c>
+      <c r="G18" s="51">
+        <v>180000</v>
+      </c>
+      <c r="H18" s="51">
+        <v>600000</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>28</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A16:A22"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A5:E5"/>
-    <mergeCell ref="A14:D14"/>
-    <mergeCell ref="B15:D15"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>